<commit_message>
further fleshing out results qmd
</commit_message>
<xml_diff>
--- a/Data/bih_postwar_municipality_metadata.xlsx
+++ b/Data/bih_postwar_municipality_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timmyballesteros/R/bih_voting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8E6DCE-312B-CE46-A644-6ED288003964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280E087C-8C04-E34A-A69C-D5F63D26958F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20880" xr2:uid="{0F486FED-49D3-C145-8825-8025B6C40CD4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$143</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -914,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59920D55-899A-7E43-BDF0-652A97E7BB88}">
   <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2705,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="E93" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
@@ -3698,6 +3698,11 @@
       <c r="E148" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E143" xr:uid="{59920D55-899A-7E43-BDF0-652A97E7BB88}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A45:E137">
+      <sortCondition ref="A1:A143"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E148">
     <sortCondition ref="A2:A148"/>
   </sortState>

</xml_diff>